<commit_message>
update all files and text
</commit_message>
<xml_diff>
--- a/merchantXlsxFiles/add-store-user.xlsx
+++ b/merchantXlsxFiles/add-store-user.xlsx
@@ -1,41 +1,125 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cashewlaptop/files/works/json-to-xslt/merchantXlsxFiles/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E6AB1CD-1552-AA48-A8C7-860309A1EB25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>addStoreUser.firstName</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>addStoreUser.lastName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>addStoreUser.emailAddress</t>
+  </si>
+  <si>
+    <t>Email address</t>
+  </si>
+  <si>
+    <t>addStoreUser.countryCode</t>
+  </si>
+  <si>
+    <t>Country code</t>
+  </si>
+  <si>
+    <t>addStoreUser.phoneNumber</t>
+  </si>
+  <si>
+    <t>Phone number</t>
+  </si>
+  <si>
+    <t>addStoreUser.assignedStore</t>
+  </si>
+  <si>
+    <t>Assigned store</t>
+  </si>
+  <si>
+    <t>addStoreUser.cancel</t>
+  </si>
+  <si>
+    <t>Cancel</t>
+  </si>
+  <si>
+    <t>addStoreUser.createStoreUser</t>
+  </si>
+  <si>
+    <t>Create store user</t>
+  </si>
+  <si>
+    <t>addStoreUser.passwordRules1</t>
+  </si>
+  <si>
+    <t>Password needs to have a minimum length of 8 characters</t>
+  </si>
+  <si>
+    <t>addStoreUser.passwordRules2</t>
+  </si>
+  <si>
+    <t>Password needs to have at least 1 lower case and 1 upper case character</t>
+  </si>
+  <si>
+    <t>addStoreUser.passwordRules3</t>
+  </si>
+  <si>
+    <t>Password needs to contain at least 1 non alphanumeric character: ~!@#$%^&amp;*_-+=|()}[]:;"&lt;&gt;,.?/{</t>
+  </si>
+  <si>
+    <t>addStoreUser.passwordRules4</t>
+  </si>
+  <si>
+    <t>Password needs to include at least 1 digit (0 - 9)</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Button</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -65,13 +149,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,119 +488,165 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="83.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>String</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Value</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>addStoreUser.firstName</v>
-      </c>
-      <c r="B2" t="str">
-        <v>FirstName</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>addStoreUser.lastName</v>
-      </c>
-      <c r="B3" t="str">
-        <v>LastName</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>addStoreUser.emailAddress</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Email address</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>addStoreUser.countryCode</v>
-      </c>
-      <c r="B5" t="str">
-        <v>Country code</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>addStoreUser.phoneNumber</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Phone number</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="str">
-        <v>addStoreUser.assignedStore</v>
-      </c>
-      <c r="B7" t="str">
-        <v>Assigned store</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>addStoreUser.cancel</v>
-      </c>
-      <c r="B8" t="str">
-        <v>Cancel</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
-        <v>addStoreUser.createStoreUser</v>
-      </c>
-      <c r="B9" t="str">
-        <v>Create store user</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>addStoreUser.passwordRules1</v>
-      </c>
-      <c r="B10" t="str">
-        <v>Password needs to have a minimum length of 8 characters</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="str">
-        <v>addStoreUser.passwordRules2</v>
-      </c>
-      <c r="B11" t="str">
-        <v>Password needs to have at least 1 lower case and 1 upper case character</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>addStoreUser.passwordRules3</v>
-      </c>
-      <c r="B12" t="str">
-        <v>Password needs to contain at least 1 non alphanumeric character: ~!@#$%^&amp;*_-+=|()}[]:;"&lt;&gt;,.?/{</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="str">
-        <v>addStoreUser.passwordRules4</v>
-      </c>
-      <c r="B13" t="str">
-        <v>Password needs to include at least 1 digit (0 - 9)</v>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B13"/>
+    <ignoredError sqref="A1:B13" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>